<commit_message>
añadidas clases de habilidades
</commit_message>
<xml_diff>
--- a/Plantilla de habilidades.xlsx
+++ b/Plantilla de habilidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UTN\2022\Lab II\pryectazo6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\Proyectos VS\Proyectazo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE13A65-9DB8-4EEE-AE2F-895DFEADF0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936493CC-57B7-4B23-9213-8DE060E502CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F289420B-928D-4B6D-9A00-B13F97946B31}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15510" windowHeight="11190" xr2:uid="{F289420B-928D-4B6D-9A00-B13F97946B31}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="109">
   <si>
     <t>Fireball</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>Fireball+Earth Armor</t>
-  </si>
-  <si>
-    <t>Hace daño de fuego y tierra</t>
   </si>
   <si>
     <t>Hace daño de tierra y PROBABILIDAD de stunear</t>
@@ -247,12 +244,6 @@
     <t>Swirl</t>
   </si>
   <si>
-    <t>Disminuye un 10% el siguiente ataque del enemigo si es de fuego.</t>
-  </si>
-  <si>
-    <t>Cura xd el 50% del daño hecho?</t>
-  </si>
-  <si>
     <t>15% EXTRAS?</t>
   </si>
   <si>
@@ -288,9 +279,6 @@
   </si>
   <si>
     <t>Bubble + Bubble</t>
-  </si>
-  <si>
-    <t>Hace 15% extra al fuego. Cura si el enemigo es de agua?</t>
   </si>
   <si>
     <t>neutral</t>
@@ -337,32 +325,152 @@
     <t>Doton</t>
   </si>
   <si>
-    <t>Stun por un turno</t>
-  </si>
-  <si>
     <t>Barrier + hab. Base de elemento</t>
   </si>
   <si>
     <t>Aumenta la defensa del tipo de elemento</t>
   </si>
   <si>
-    <t>Ignora escudos(? Hay escudos? Xd</t>
-  </si>
-  <si>
-    <t>10% de resistencia a todos los elementos (O ESCUDO?)</t>
-  </si>
-  <si>
-    <t>INSERTEUNNOMBRE</t>
-  </si>
-  <si>
-    <t>windoblow + earth armor</t>
+    <t>Hace daño verdadero</t>
+  </si>
+  <si>
+    <t>Sabaku Kyu</t>
+  </si>
+  <si>
+    <t>el cura que cura</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>uso de mp</t>
+  </si>
+  <si>
+    <t>yo</t>
+  </si>
+  <si>
+    <t>windoblows + earth armor</t>
+  </si>
+  <si>
+    <t>Hace daño x2 a los enemigos de fuego</t>
+  </si>
+  <si>
+    <t>Disminuye un 20% el siguiente ataque del enemigo.</t>
+  </si>
+  <si>
+    <t>Aumenta la defensa física</t>
+  </si>
+  <si>
+    <t>Ataques</t>
+  </si>
+  <si>
+    <t>Habilidades</t>
+  </si>
+  <si>
+    <t>10% de resistencia a todos los elementos y los ataques básicos hacen daño de tierra</t>
+  </si>
+  <si>
+    <t>Columna1</t>
+  </si>
+  <si>
+    <t>Columna2</t>
+  </si>
+  <si>
+    <t>Columna3</t>
+  </si>
+  <si>
+    <t>Columna4</t>
+  </si>
+  <si>
+    <t>Columna5</t>
+  </si>
+  <si>
+    <t>Columna6</t>
+  </si>
+  <si>
+    <t>Columna7</t>
+  </si>
+  <si>
+    <t>DamageMultiplier</t>
+  </si>
+  <si>
+    <t>Vampirismo</t>
+  </si>
+  <si>
+    <t>StunProb</t>
+  </si>
+  <si>
+    <t>Por 1 turno</t>
+  </si>
+  <si>
+    <t>Hace daño y reduce la defensa mágica</t>
+  </si>
+  <si>
+    <t>reducePD</t>
+  </si>
+  <si>
+    <t>reduceMR</t>
+  </si>
+  <si>
+    <t>Hace daño y reduce la defensa física</t>
+  </si>
+  <si>
+    <t>burn</t>
+  </si>
+  <si>
+    <t>poison</t>
+  </si>
+  <si>
+    <t>reduceAtt</t>
+  </si>
+  <si>
+    <t>truedamash</t>
+  </si>
+  <si>
+    <t>risePD</t>
+  </si>
+  <si>
+    <t>riseMR</t>
+  </si>
+  <si>
+    <t>heal</t>
+  </si>
+  <si>
+    <t>statusHeal</t>
+  </si>
+  <si>
+    <t>elementMR</t>
+  </si>
+  <si>
+    <t>mirror</t>
+  </si>
+  <si>
+    <t>elementAtt</t>
+  </si>
+  <si>
+    <t>:(</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>como controlar los turnos correctamente</t>
+  </si>
+  <si>
+    <t>terminar los sets y gets de las habilidades</t>
+  </si>
+  <si>
+    <t>como PINGO hacer funcionar el vampirismo</t>
+  </si>
+  <si>
+    <t>^^quelenemigotecure^.^</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,8 +529,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -453,6 +576,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -466,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -505,11 +634,42 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -754,6 +914,22 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A3ACF86-7AC4-4CCC-B8D5-9493EDCB2A22}" name="Tabla1" displayName="Tabla1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:G22" xr:uid="{4A3ACF86-7AC4-4CCC-B8D5-9493EDCB2A22}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{5E818E1B-7B67-4330-9694-CF50496B1827}" name="Columna1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{18395091-2274-49A8-B58A-8BD688DEE5C6}" name="Columna2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{2BD207E8-08B9-426F-B378-F1F4CFF63F78}" name="Columna3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{931F7E68-7FFC-421D-A4E2-5EF53D6C464B}" name="Columna4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{9DE6B76A-1451-486E-B6FC-1B155619E8C3}" name="Columna5"/>
+    <tableColumn id="6" xr3:uid="{80DC395C-337E-49E0-92D0-A61FEBBB9F85}" name="Columna6" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{DC8CDE1A-2E14-4C8F-9EAA-CABB3F1E9228}" name="Columna7" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1053,10 +1229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1575B6-EC1A-4D1D-8BD4-746F0EB28CFF}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="F15" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,374 +1240,577 @@
     <col min="1" max="1" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="71.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="G3" s="1">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>73</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>53</v>
+        <v>25</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>41</v>
+        <v>66</v>
+      </c>
+      <c r="G8" s="1">
+        <v>5</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>68</v>
+        <v>40</v>
+      </c>
+      <c r="G9" s="1">
+        <v>15</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>29</v>
+        <v>63</v>
+      </c>
+      <c r="G10" s="1">
+        <v>10</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="F12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>62</v>
+        <v>12</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <v>25</v>
+      </c>
+      <c r="M14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="M15">
+        <v>25</v>
+      </c>
+      <c r="N15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="K16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="E19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="1">
         <v>30</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="3" t="s">
+    </row>
+    <row r="20" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="F20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G21" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>84</v>
+      </c>
+      <c r="I25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>85</v>
+      </c>
+      <c r="I26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H27" t="s">
+        <v>86</v>
+      </c>
+      <c r="I27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H28" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H29" t="s">
+        <v>90</v>
+      </c>
+      <c r="I29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" t="s">
+        <v>92</v>
+      </c>
+      <c r="I30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>93</v>
+      </c>
+      <c r="I31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mejoradas las clases de habilidades
</commit_message>
<xml_diff>
--- a/Plantilla de habilidades.xlsx
+++ b/Plantilla de habilidades.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\Proyectos VS\Proyectazo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\Backup Lucas Junio - 2022\Proyectos VS\Proyectazo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936493CC-57B7-4B23-9213-8DE060E502CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488D288B-65AB-4C70-8EAA-A5D1E88D90C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15510" windowHeight="11190" xr2:uid="{F289420B-928D-4B6D-9A00-B13F97946B31}"/>
+    <workbookView xWindow="10425" yWindow="3930" windowWidth="15510" windowHeight="11190" activeTab="1" xr2:uid="{F289420B-928D-4B6D-9A00-B13F97946B31}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="121">
   <si>
     <t>Fireball</t>
   </si>
@@ -464,6 +465,42 @@
   </si>
   <si>
     <t>^^quelenemigotecure^.^</t>
+  </si>
+  <si>
+    <t>AbilityFactory</t>
+  </si>
+  <si>
+    <t>EnemyFactory</t>
+  </si>
+  <si>
+    <t>Enemy enemy;</t>
+  </si>
+  <si>
+    <t>Ability ability;</t>
+  </si>
+  <si>
+    <t>set stats</t>
+  </si>
+  <si>
+    <t>set habilidad 1</t>
+  </si>
+  <si>
+    <t>set habilidad 2</t>
+  </si>
+  <si>
+    <t>set sprite</t>
+  </si>
+  <si>
+    <t>Quei simo</t>
+  </si>
+  <si>
+    <t>Dragon checkstates()</t>
+  </si>
+  <si>
+    <t>kea ser</t>
+  </si>
+  <si>
+    <t>definir lo que hay que hacer con useAbility (relación con checkstates());</t>
   </si>
 </sst>
 </file>
@@ -649,13 +686,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -917,16 +954,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A3ACF86-7AC4-4CCC-B8D5-9493EDCB2A22}" name="Tabla1" displayName="Tabla1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A3ACF86-7AC4-4CCC-B8D5-9493EDCB2A22}" name="Tabla1" displayName="Tabla1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:G22" xr:uid="{4A3ACF86-7AC4-4CCC-B8D5-9493EDCB2A22}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5E818E1B-7B67-4330-9694-CF50496B1827}" name="Columna1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{18395091-2274-49A8-B58A-8BD688DEE5C6}" name="Columna2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{2BD207E8-08B9-426F-B378-F1F4CFF63F78}" name="Columna3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{931F7E68-7FFC-421D-A4E2-5EF53D6C464B}" name="Columna4" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{5E818E1B-7B67-4330-9694-CF50496B1827}" name="Columna1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{18395091-2274-49A8-B58A-8BD688DEE5C6}" name="Columna2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{2BD207E8-08B9-426F-B378-F1F4CFF63F78}" name="Columna3" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{931F7E68-7FFC-421D-A4E2-5EF53D6C464B}" name="Columna4" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{9DE6B76A-1451-486E-B6FC-1B155619E8C3}" name="Columna5"/>
-    <tableColumn id="6" xr3:uid="{80DC395C-337E-49E0-92D0-A61FEBBB9F85}" name="Columna6" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{DC8CDE1A-2E14-4C8F-9EAA-CABB3F1E9228}" name="Columna7" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{80DC395C-337E-49E0-92D0-A61FEBBB9F85}" name="Columna6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{DC8CDE1A-2E14-4C8F-9EAA-CABB3F1E9228}" name="Columna7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1231,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1575B6-EC1A-4D1D-8BD4-746F0EB28CFF}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F15" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,4 +1850,178 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9076AE7E-FB59-4599-805D-C36A527D9B9A}">
+  <dimension ref="B3:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>3425</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>345</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="I25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>34234</v>
+      </c>
+      <c r="E26">
+        <v>52</v>
+      </c>
+      <c r="F26">
+        <v>345</v>
+      </c>
+      <c r="G26">
+        <v>2345</v>
+      </c>
+      <c r="H26">
+        <v>23</v>
+      </c>
+      <c r="I26">
+        <v>4523</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>52</v>
+      </c>
+      <c r="E27">
+        <v>324</v>
+      </c>
+      <c r="F27">
+        <v>63</v>
+      </c>
+      <c r="G27">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>56</v>
+      </c>
+      <c r="F28">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>